<commit_message>
commit mau bao cao
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/BaoCao/Thong_Ke_So_Luong_Hoa_Don_Da_Phat_Hanh.xlsx
+++ b/API/wwwroot/docs/BaoCao/Thong_Ke_So_Luong_Hoa_Don_Da_Phat_Hanh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\bill-back-end\API\wwwroot\docs\BaoCao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7242F809-894E-4B07-88AE-341446F96B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47E919D-326E-429F-868F-A20F8B211FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,7 +126,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,29 +241,8 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -271,6 +256,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,129 +624,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="82.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="82.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="9" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
them xuat khau tinh hinh sd hoa don
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/BaoCao/Thong_Ke_So_Luong_Hoa_Don_Da_Phat_Hanh.xlsx
+++ b/API/wwwroot/docs/BaoCao/Thong_Ke_So_Luong_Hoa_Don_Da_Phat_Hanh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\bill-back-end\API\wwwroot\docs\BaoCao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6148E5-8D54-4F5E-8C36-A3F7D846E973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485F76EF-AE91-49B3-8244-F6B4D5362576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -626,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -636,9 +636,9 @@
     <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="47.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>